<commit_message>
Add credit hour totals to flow chart. Revise course load to reflect credit hour overage. Add some courses to the Work Units spreadsheet.
</commit_message>
<xml_diff>
--- a/assets/Work Units.xlsx
+++ b/assets/Work Units.xlsx
@@ -1,43 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\fiscal\Shared\Accounting\Program Planning\Program Expansion Committee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongbakos/projects/bsse/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26505" windowHeight="11385"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="51120" windowHeight="31540"/>
   </bookViews>
   <sheets>
     <sheet name="Course List" sheetId="1" r:id="rId1"/>
     <sheet name="Tables" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Course List'!$A$1:$J$73</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Course List'!$E$71:$E$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Course List'!$A$1:$J$72</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Course List'!$E$70:$E$71</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Course List'!$G$74</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Course List'!$G$74</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Course List'!$G$74</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Course List'!$G$73</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Course List'!$G$73</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Course List'!$G$73</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Course List'!$E$73</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Course List'!$E$72</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Course List'!$G$67</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Course List'!$G$67</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Course List'!$G$67</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Course List'!$G$66</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Course List'!$G$66</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Course List'!$G$66</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -45,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="122">
   <si>
     <t>Agriculture</t>
   </si>
@@ -363,12 +369,66 @@
   </si>
   <si>
     <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>SE 101</t>
+  </si>
+  <si>
+    <t>SE 102</t>
+  </si>
+  <si>
+    <t>SE 103</t>
+  </si>
+  <si>
+    <t>Creative Coding I</t>
+  </si>
+  <si>
+    <t>Creative Coding II</t>
+  </si>
+  <si>
+    <t>Creative Coding III</t>
+  </si>
+  <si>
+    <t>SE 111</t>
+  </si>
+  <si>
+    <t>SE 112</t>
+  </si>
+  <si>
+    <t>SE 113</t>
+  </si>
+  <si>
+    <t>Introduction to Software Engineering I</t>
+  </si>
+  <si>
+    <t>Introduction to Software Engineering II</t>
+  </si>
+  <si>
+    <t>Introduction to Software Engineering III</t>
+  </si>
+  <si>
+    <t>SE 121</t>
+  </si>
+  <si>
+    <t>Professional Seminar</t>
+  </si>
+  <si>
+    <t>SE 122</t>
+  </si>
+  <si>
+    <t>SE 123</t>
+  </si>
+  <si>
+    <t>SE 124</t>
+  </si>
+  <si>
+    <t>Apprenticeship I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0_);\(#,##0.0\)"/>
     <numFmt numFmtId="165" formatCode="0.0_);\(0.0\)"/>
@@ -542,14 +602,14 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,10 +617,10 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,10 +632,10 @@
         <color rgb="FF7F7F7F"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,19 +644,19 @@
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -606,7 +666,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -617,7 +677,7 @@
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
@@ -638,7 +698,7 @@
         <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,19 +707,19 @@
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF3F3F3F"/>
@@ -674,7 +734,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FF3F3F3F"/>
@@ -683,7 +743,7 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -698,17 +758,17 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -717,7 +777,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -725,22 +785,22 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,37 +815,37 @@
         <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -967,9 +1027,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1002,9 +1062,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1184,30 +1244,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="44.42578125" customWidth="1"/>
+    <col min="4" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
@@ -1226,7 +1286,7 @@
       <c r="J1" s="51"/>
       <c r="K1" s="48"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1239,7 +1299,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1254,7 +1314,7 @@
       <c r="J3" s="47"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1267,7 +1327,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>91</v>
       </c>
@@ -1300,7 +1360,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>76</v>
       </c>
@@ -1333,18 +1393,26 @@
       </c>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>107</v>
+      </c>
       <c r="C7" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D7" s="19">
+        <v>2</v>
+      </c>
       <c r="E7" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="19">
+        <v>1</v>
+      </c>
       <c r="H7" s="19">
         <f>IF(I7="Select",1,0)</f>
         <v>1</v>
@@ -1357,20 +1425,28 @@
       </c>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="C8" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D8" s="19">
+        <v>2</v>
+      </c>
       <c r="E8" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
+      <c r="G8" s="19">
+        <v>1</v>
+      </c>
       <c r="H8" s="19">
-        <f t="shared" ref="H8:H65" si="0">IF(I8="Select",1,0)</f>
+        <f t="shared" ref="H8:H64" si="0">IF(I8="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I8" s="21" t="s">
@@ -1381,18 +1457,26 @@
       </c>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>109</v>
+      </c>
       <c r="C9" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D9" s="19">
+        <v>2</v>
+      </c>
       <c r="E9" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
+      <c r="G9" s="19">
+        <v>1</v>
+      </c>
       <c r="H9" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1405,18 +1489,26 @@
       </c>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>113</v>
+      </c>
       <c r="C10" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D10" s="19">
+        <v>8</v>
+      </c>
       <c r="E10" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F10" s="20"/>
-      <c r="G10" s="19"/>
+      <c r="G10" s="19">
+        <v>1</v>
+      </c>
       <c r="H10" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1429,18 +1521,26 @@
       </c>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="C11" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D11" s="19">
+        <v>8</v>
+      </c>
       <c r="E11" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F11" s="20"/>
-      <c r="G11" s="19"/>
+      <c r="G11" s="19">
+        <v>1</v>
+      </c>
       <c r="H11" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1453,18 +1553,26 @@
       </c>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>115</v>
+      </c>
       <c r="C12" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D12" s="19">
+        <v>8</v>
+      </c>
       <c r="E12" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="19"/>
+      <c r="G12" s="19">
+        <v>1</v>
+      </c>
       <c r="H12" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1477,18 +1585,26 @@
       </c>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>117</v>
+      </c>
       <c r="C13" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D13" s="19">
+        <v>1</v>
+      </c>
       <c r="E13" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F13" s="20"/>
-      <c r="G13" s="19"/>
+      <c r="G13" s="19">
+        <v>1</v>
+      </c>
       <c r="H13" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1501,15 +1617,21 @@
       </c>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>121</v>
+      </c>
       <c r="C14" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D14" s="19">
+        <v>1</v>
+      </c>
       <c r="E14" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="19"/>
@@ -1525,15 +1647,21 @@
       </c>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>121</v>
+      </c>
       <c r="C15" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D15" s="19">
+        <v>1</v>
+      </c>
       <c r="E15" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="19"/>
@@ -1549,13 +1677,19 @@
       </c>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>121</v>
+      </c>
       <c r="C16" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D16" s="19">
+        <v>1</v>
+      </c>
       <c r="E16" s="21" t="s">
         <v>71</v>
       </c>
@@ -1573,7 +1707,7 @@
       </c>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="21" t="s">
@@ -1597,7 +1731,7 @@
       </c>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="21" t="s">
@@ -1621,7 +1755,7 @@
       </c>
       <c r="K18" s="22"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="21" t="s">
@@ -1645,7 +1779,7 @@
       </c>
       <c r="K19" s="22"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="21" t="s">
@@ -1669,7 +1803,7 @@
       </c>
       <c r="K20" s="22"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="21" t="s">
@@ -1693,7 +1827,7 @@
       </c>
       <c r="K21" s="22"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="21" t="s">
@@ -1717,7 +1851,7 @@
       </c>
       <c r="K22" s="22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="21" t="s">
@@ -1741,7 +1875,7 @@
       </c>
       <c r="K23" s="22"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="21" t="s">
@@ -1765,7 +1899,7 @@
       </c>
       <c r="K24" s="22"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="21" t="s">
@@ -1789,7 +1923,7 @@
       </c>
       <c r="K25" s="22"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="21" t="s">
@@ -1813,7 +1947,7 @@
       </c>
       <c r="K26" s="22"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="21" t="s">
@@ -1837,7 +1971,7 @@
       </c>
       <c r="K27" s="22"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="21" t="s">
@@ -1861,7 +1995,7 @@
       </c>
       <c r="K28" s="22"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="21" t="s">
@@ -1885,7 +2019,7 @@
       </c>
       <c r="K29" s="22"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="21" t="s">
@@ -1909,7 +2043,7 @@
       </c>
       <c r="K30" s="22"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="21" t="s">
@@ -1933,7 +2067,7 @@
       </c>
       <c r="K31" s="22"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="21" t="s">
@@ -1957,7 +2091,7 @@
       </c>
       <c r="K32" s="22"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="18"/>
       <c r="C33" s="21" t="s">
@@ -1981,7 +2115,7 @@
       </c>
       <c r="K33" s="22"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="21" t="s">
@@ -2005,7 +2139,7 @@
       </c>
       <c r="K34" s="22"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="21" t="s">
@@ -2029,7 +2163,7 @@
       </c>
       <c r="K35" s="22"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
       <c r="C36" s="21" t="s">
@@ -2053,7 +2187,7 @@
       </c>
       <c r="K36" s="22"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="18"/>
       <c r="C37" s="21" t="s">
@@ -2077,7 +2211,7 @@
       </c>
       <c r="K37" s="22"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="21" t="s">
@@ -2101,7 +2235,7 @@
       </c>
       <c r="K38" s="22"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="21" t="s">
@@ -2125,7 +2259,7 @@
       </c>
       <c r="K39" s="22"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="18"/>
       <c r="C40" s="21" t="s">
@@ -2149,7 +2283,7 @@
       </c>
       <c r="K40" s="22"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="18"/>
       <c r="C41" s="21" t="s">
@@ -2173,7 +2307,7 @@
       </c>
       <c r="K41" s="22"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="21" t="s">
@@ -2197,7 +2331,7 @@
       </c>
       <c r="K42" s="22"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="18"/>
       <c r="C43" s="21" t="s">
@@ -2221,7 +2355,7 @@
       </c>
       <c r="K43" s="22"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="18"/>
       <c r="C44" s="21" t="s">
@@ -2245,7 +2379,7 @@
       </c>
       <c r="K44" s="22"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="18"/>
       <c r="C45" s="21" t="s">
@@ -2269,7 +2403,7 @@
       </c>
       <c r="K45" s="22"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="18"/>
       <c r="C46" s="21" t="s">
@@ -2293,7 +2427,7 @@
       </c>
       <c r="K46" s="22"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="18"/>
       <c r="C47" s="21" t="s">
@@ -2317,7 +2451,7 @@
       </c>
       <c r="K47" s="22"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="18"/>
       <c r="C48" s="21" t="s">
@@ -2341,7 +2475,7 @@
       </c>
       <c r="K48" s="22"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="18"/>
       <c r="C49" s="21" t="s">
@@ -2365,7 +2499,7 @@
       </c>
       <c r="K49" s="22"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="18"/>
       <c r="C50" s="21" t="s">
@@ -2389,7 +2523,7 @@
       </c>
       <c r="K50" s="22"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="18"/>
       <c r="C51" s="21" t="s">
@@ -2413,7 +2547,7 @@
       </c>
       <c r="K51" s="22"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="18"/>
       <c r="C52" s="21" t="s">
@@ -2437,7 +2571,7 @@
       </c>
       <c r="K52" s="22"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
       <c r="B53" s="18"/>
       <c r="C53" s="21" t="s">
@@ -2461,7 +2595,7 @@
       </c>
       <c r="K53" s="22"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
       <c r="B54" s="18"/>
       <c r="C54" s="21" t="s">
@@ -2485,7 +2619,7 @@
       </c>
       <c r="K54" s="22"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
       <c r="B55" s="18"/>
       <c r="C55" s="21" t="s">
@@ -2509,7 +2643,7 @@
       </c>
       <c r="K55" s="22"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
       <c r="B56" s="18"/>
       <c r="C56" s="21" t="s">
@@ -2533,7 +2667,7 @@
       </c>
       <c r="K56" s="22"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="B57" s="18"/>
       <c r="C57" s="21" t="s">
@@ -2557,7 +2691,7 @@
       </c>
       <c r="K57" s="22"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="17"/>
       <c r="B58" s="18"/>
       <c r="C58" s="21" t="s">
@@ -2581,7 +2715,7 @@
       </c>
       <c r="K58" s="22"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
       <c r="B59" s="18"/>
       <c r="C59" s="21" t="s">
@@ -2605,7 +2739,7 @@
       </c>
       <c r="K59" s="22"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="17"/>
       <c r="B60" s="18"/>
       <c r="C60" s="21" t="s">
@@ -2629,7 +2763,7 @@
       </c>
       <c r="K60" s="22"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="17"/>
       <c r="B61" s="18"/>
       <c r="C61" s="21" t="s">
@@ -2653,7 +2787,7 @@
       </c>
       <c r="K61" s="22"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="17"/>
       <c r="B62" s="18"/>
       <c r="C62" s="21" t="s">
@@ -2677,7 +2811,7 @@
       </c>
       <c r="K62" s="22"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="18"/>
       <c r="C63" s="21" t="s">
@@ -2701,180 +2835,176 @@
       </c>
       <c r="K63" s="22"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F64" s="20"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I64" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="J64" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="K64" s="22"/>
-    </row>
-    <row r="65" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="23"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D65" s="25"/>
-      <c r="E65" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F65" s="26"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I65" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="J65" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="K65" s="46"/>
-    </row>
-    <row r="66" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C67" s="12" t="s">
+    <row r="64" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="25"/>
+      <c r="E64" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="26"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I64" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="J64" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K64" s="46"/>
+    </row>
+    <row r="65" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:16" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D67" s="29">
-        <f>SUM(D6:D65)</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="12" t="s">
+      <c r="D66" s="29">
+        <f>SUM(D6:D64)</f>
+        <v>34</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G67" s="11">
-        <f>SUMPRODUCT(F6:F65,G6:G65,H6:H65)</f>
+      <c r="G66" s="11">
+        <f>SUMPRODUCT(F6:F64,G6:G64,H6:H64)</f>
         <v>3.5</v>
       </c>
-      <c r="M67" s="15"/>
-    </row>
-    <row r="68" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D69" s="37" t="s">
+      <c r="M66" s="15"/>
+    </row>
+    <row r="67" spans="1:16" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D68" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="39"/>
-    </row>
-    <row r="70" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="D70" s="4"/>
-      <c r="E70" s="30" t="s">
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="39"/>
+    </row>
+    <row r="69" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+      <c r="D69" s="4"/>
+      <c r="E69" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="F69" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="G70" s="32" t="s">
+      <c r="G69" s="32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
+      <c r="D70" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="42">
+        <f>SUMIF(E75:E83,"TT",B75:B83)</f>
+        <v>3.5</v>
+      </c>
+      <c r="F70" s="34">
+        <f>E70/21</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G70" s="40"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
       <c r="D71" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E71" s="42">
-        <f>SUMIF(E76:E84,"TT",B76:B84)</f>
+        <f>SUMIF(E75:E83,"Instructor",B75:B83)</f>
+        <v>0</v>
+      </c>
+      <c r="F71" s="34">
+        <f>E71/28</f>
+        <v>0</v>
+      </c>
+      <c r="G71" s="40"/>
+      <c r="P71" s="13"/>
+    </row>
+    <row r="72" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="D72" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E72" s="43">
+        <f>G66-E70-E71</f>
+        <v>0</v>
+      </c>
+      <c r="F72" s="36">
+        <f>E72</f>
+        <v>0</v>
+      </c>
+      <c r="G72" s="41"/>
+    </row>
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="16">
+        <f t="shared" ref="A75:A83" si="1">C75/D75</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="B75" s="14">
+        <f>IF(G66=3.5,3.5,IF(A75&lt;0.5,0,IF(AND(A75&gt;=0.5,A75&lt;=1),C75,D75)))</f>
         <v>3.5</v>
       </c>
-      <c r="F71" s="34">
-        <f>E71/21</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G71" s="40"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="D72" s="33" t="s">
+      <c r="C75">
+        <f>G66</f>
+        <v>3.5</v>
+      </c>
+      <c r="D75">
+        <v>21</v>
+      </c>
+      <c r="E75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B76" s="14">
+        <f t="shared" ref="B76:B83" si="2">IF(B75=0,0,IF(A76&lt;0.5,0,IF(AND(A76&gt;=0.5,A76&lt;=1),C76,D76)))</f>
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <f>G66-B75</f>
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>28</v>
+      </c>
+      <c r="E76" t="s">
         <v>80</v>
       </c>
-      <c r="E72" s="42">
-        <f>SUMIF(E76:E84,"Instructor",B76:B84)</f>
-        <v>0</v>
-      </c>
-      <c r="F72" s="34">
-        <f>E72/28</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="40"/>
-      <c r="P72" s="13"/>
-    </row>
-    <row r="73" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="5"/>
-      <c r="D73" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="E73" s="43">
-        <f>G67-E71-E72</f>
-        <v>0</v>
-      </c>
-      <c r="F73" s="36">
-        <f>E73</f>
-        <v>0</v>
-      </c>
-      <c r="G73" s="41"/>
-    </row>
-    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="16">
-        <f t="shared" ref="A76:A84" si="1">C76/D76</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="B76" s="14">
-        <f>IF(G67=3.5,3.5,IF(A76&lt;0.5,0,IF(AND(A76&gt;=0.5,A76&lt;=1),C76,D76)))</f>
-        <v>3.5</v>
-      </c>
-      <c r="C76">
-        <f>G67</f>
-        <v>3.5</v>
-      </c>
-      <c r="D76">
-        <v>21</v>
-      </c>
-      <c r="E76" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="B77" s="14">
-        <f t="shared" ref="B77:B84" si="2">IF(B76=0,0,IF(A77&lt;0.5,0,IF(AND(A77&gt;=0.5,A77&lt;=1),C77,D77)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C77">
-        <f>G67-B76</f>
+        <f>G66-B75-B76</f>
         <v>0</v>
       </c>
       <c r="D77">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E77" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2884,17 +3014,17 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <f>G67-B76-B77</f>
+        <f>G66-B75-B76-B77</f>
         <v>0</v>
       </c>
       <c r="D78">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E78" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2904,17 +3034,17 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <f>G67-B76-B77-B78</f>
+        <f>G66-B75-B76-B77-B78</f>
         <v>0</v>
       </c>
       <c r="D79">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E79" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2924,17 +3054,17 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <f>G67-B76-B77-B78-B79</f>
+        <f>G66-B75-B76-B77-B78-B79</f>
         <v>0</v>
       </c>
       <c r="D80">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2944,17 +3074,17 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <f>G67-B76-B77-B78-B79-B80</f>
+        <f>G66-B75-B76-B77-B78-B79-B80</f>
         <v>0</v>
       </c>
       <c r="D81">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2964,17 +3094,17 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <f>G67-B76-B77-B78-B79-B80-B81</f>
+        <f>G66-B75-B76-B77-B78-B79-B80-B81</f>
         <v>0</v>
       </c>
       <c r="D82">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E82" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2984,33 +3114,13 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <f>G67-B76-B77-B78-B79-B80-B81-B82</f>
+        <f>G66-B75-B76-B77-B78-B79-B80-B81-B82</f>
         <v>0</v>
       </c>
       <c r="D83">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E83" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B84" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C84">
-        <f>G67-B76-B77-B78-B79-B80-B81-B82-B83</f>
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>21</v>
-      </c>
-      <c r="E84" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3031,19 +3141,19 @@
           <x14:formula1>
             <xm:f>Tables!$D$1:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E7:E65</xm:sqref>
+          <xm:sqref>E7:E64</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$E$1:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C65</xm:sqref>
+          <xm:sqref>C7:C64</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$A$1:$A$72</xm:f>
           </x14:formula1>
-          <xm:sqref>I7:J65</xm:sqref>
+          <xm:sqref>I7:J64</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3053,7 +3163,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:E72"/>
@@ -3062,14 +3172,14 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -3083,7 +3193,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -3097,7 +3207,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -3111,7 +3221,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3122,7 +3232,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -3130,7 +3240,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -3138,7 +3248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -3146,7 +3256,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -3154,7 +3264,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3162,7 +3272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3170,7 +3280,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3178,7 +3288,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3186,7 +3296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -3194,7 +3304,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -3202,7 +3312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -3210,7 +3320,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3218,7 +3328,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3226,7 +3336,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3234,7 +3344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3242,7 +3352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -3250,7 +3360,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -3258,7 +3368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -3266,7 +3376,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -3274,7 +3384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -3282,7 +3392,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -3290,7 +3400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -3298,7 +3408,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -3306,7 +3416,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -3314,7 +3424,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -3322,7 +3432,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -3330,7 +3440,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3338,7 +3448,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3346,7 +3456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -3354,7 +3464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -3362,7 +3472,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -3370,7 +3480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3378,7 +3488,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -3386,7 +3496,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -3394,7 +3504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -3402,7 +3512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -3410,7 +3520,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -3418,7 +3528,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -3426,7 +3536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -3434,7 +3544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -3442,7 +3552,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -3450,7 +3560,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -3458,7 +3568,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -3466,7 +3576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -3474,7 +3584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -3482,7 +3592,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>27</v>
       </c>
@@ -3490,7 +3600,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -3498,7 +3608,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -3506,7 +3616,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -3514,7 +3624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>45</v>
       </c>
@@ -3522,7 +3632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -3530,7 +3640,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -3538,7 +3648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -3546,7 +3656,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -3554,7 +3664,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -3562,7 +3672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -3570,7 +3680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -3578,7 +3688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>47</v>
       </c>
@@ -3586,7 +3696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>31</v>
       </c>
@@ -3594,7 +3704,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>32</v>
       </c>
@@ -3602,7 +3712,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>37</v>
       </c>
@@ -3610,7 +3720,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -3618,7 +3728,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -3626,7 +3736,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -3634,7 +3744,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -3642,7 +3752,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -3650,7 +3760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>52</v>
       </c>
@@ -3658,7 +3768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Add final courses to work units spreadsheet.
</commit_message>
<xml_diff>
--- a/assets/Work Units.xlsx
+++ b/assets/Work Units.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="51120" windowHeight="31540"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="26380" windowHeight="20180"/>
   </bookViews>
   <sheets>
     <sheet name="Course List" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="194">
   <si>
     <t>Agriculture</t>
   </si>
@@ -380,15 +380,6 @@
     <t>SE 103</t>
   </si>
   <si>
-    <t>Creative Coding I</t>
-  </si>
-  <si>
-    <t>Creative Coding II</t>
-  </si>
-  <si>
-    <t>Creative Coding III</t>
-  </si>
-  <si>
     <t>SE 111</t>
   </si>
   <si>
@@ -407,22 +398,247 @@
     <t>Introduction to Software Engineering III</t>
   </si>
   <si>
-    <t>SE 121</t>
-  </si>
-  <si>
     <t>Professional Seminar</t>
   </si>
   <si>
-    <t>SE 122</t>
-  </si>
-  <si>
-    <t>SE 123</t>
-  </si>
-  <si>
-    <t>SE 124</t>
-  </si>
-  <si>
     <t>Apprenticeship I</t>
+  </si>
+  <si>
+    <t>Creative Problem Solving with Code I</t>
+  </si>
+  <si>
+    <t>Creative Problem Solving with Code II</t>
+  </si>
+  <si>
+    <t>Creative Problem Solving with Code III</t>
+  </si>
+  <si>
+    <t>SE 107</t>
+  </si>
+  <si>
+    <t>SE 110</t>
+  </si>
+  <si>
+    <t>WR 121</t>
+  </si>
+  <si>
+    <t>English Composition</t>
+  </si>
+  <si>
+    <t>MTH 112</t>
+  </si>
+  <si>
+    <t>Elementary Functions</t>
+  </si>
+  <si>
+    <t>Public Speaking</t>
+  </si>
+  <si>
+    <t>SE 211</t>
+  </si>
+  <si>
+    <t>SE 212</t>
+  </si>
+  <si>
+    <t>Data Science Engineering I</t>
+  </si>
+  <si>
+    <t>Data Science Engineering II</t>
+  </si>
+  <si>
+    <t>Data Science Engineering III</t>
+  </si>
+  <si>
+    <t>SE 213</t>
+  </si>
+  <si>
+    <t>SE 210</t>
+  </si>
+  <si>
+    <t>Apprenticeship II</t>
+  </si>
+  <si>
+    <t>SE 301</t>
+  </si>
+  <si>
+    <t>Elements of Computing Systems I</t>
+  </si>
+  <si>
+    <t>SE 302</t>
+  </si>
+  <si>
+    <t>SE 303</t>
+  </si>
+  <si>
+    <t>Elements of Computing Systems II</t>
+  </si>
+  <si>
+    <t>Elements of Computing Systems III</t>
+  </si>
+  <si>
+    <t>SE 311</t>
+  </si>
+  <si>
+    <t>SE 312</t>
+  </si>
+  <si>
+    <t>SE 313</t>
+  </si>
+  <si>
+    <t>Scalability, Infrastructure and Security I</t>
+  </si>
+  <si>
+    <t>Scalability, Infrastructure and Security II</t>
+  </si>
+  <si>
+    <t>Scalability, Infrastructure and Security III</t>
+  </si>
+  <si>
+    <t>SE 310</t>
+  </si>
+  <si>
+    <t>Apprenticeship III</t>
+  </si>
+  <si>
+    <t>SE 410</t>
+  </si>
+  <si>
+    <t>Apprenticeship IV</t>
+  </si>
+  <si>
+    <t>SE 411</t>
+  </si>
+  <si>
+    <t>SE 412</t>
+  </si>
+  <si>
+    <t>SE 413</t>
+  </si>
+  <si>
+    <t>Business of Software I</t>
+  </si>
+  <si>
+    <t>Business of Software II</t>
+  </si>
+  <si>
+    <t>Business of Software III</t>
+  </si>
+  <si>
+    <t>HHS 231</t>
+  </si>
+  <si>
+    <t>Lifetime Fitness for Health</t>
+  </si>
+  <si>
+    <t>PAC XXX</t>
+  </si>
+  <si>
+    <t>(Various Physical Activity Courses)</t>
+  </si>
+  <si>
+    <t>CS 391</t>
+  </si>
+  <si>
+    <t>Social and Ethical Issues in Computer Science</t>
+  </si>
+  <si>
+    <t>WR 327</t>
+  </si>
+  <si>
+    <t>Technical Writing</t>
+  </si>
+  <si>
+    <t>ST 351</t>
+  </si>
+  <si>
+    <t>Intro to Statistical Methods</t>
+  </si>
+  <si>
+    <t>BIO XXX</t>
+  </si>
+  <si>
+    <t>(Biology with Lab)</t>
+  </si>
+  <si>
+    <t>ST 352</t>
+  </si>
+  <si>
+    <t>PH XXX</t>
+  </si>
+  <si>
+    <t>(Physics with Lab)</t>
+  </si>
+  <si>
+    <t>MTH 231</t>
+  </si>
+  <si>
+    <t>Elements of Discrete Mathematics</t>
+  </si>
+  <si>
+    <t>BIO/PH XXX</t>
+  </si>
+  <si>
+    <t>(Bio or Phys Sci w/ Lab)</t>
+  </si>
+  <si>
+    <t>CS 261</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Western Culture</t>
+  </si>
+  <si>
+    <t>3 or 4</t>
+  </si>
+  <si>
+    <t>CS 271</t>
+  </si>
+  <si>
+    <t>Computer Architecture &amp; Assembly Language</t>
+  </si>
+  <si>
+    <t>Cultural Diversity</t>
+  </si>
+  <si>
+    <t>CS 381</t>
+  </si>
+  <si>
+    <t>Programming Language Fundamentals</t>
+  </si>
+  <si>
+    <t>Literature &amp; Arts</t>
+  </si>
+  <si>
+    <t>CS 325</t>
+  </si>
+  <si>
+    <t>Analysis of Algorithms</t>
+  </si>
+  <si>
+    <t>Difference, Power &amp; Discrimination</t>
+  </si>
+  <si>
+    <t>CS 344</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>Synthesis, Contemporary Global Issues</t>
+  </si>
+  <si>
+    <t>CS XXX</t>
+  </si>
+  <si>
+    <t>(Upper-division CS elective)</t>
+  </si>
+  <si>
+    <t>Social Process &amp; Intitutions</t>
+  </si>
+  <si>
+    <t>COMM 111</t>
   </si>
 </sst>
 </file>
@@ -1250,9 +1466,9 @@
   </sheetPr>
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1311,7 +1527,9 @@
       <c r="I3" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="J3" s="47"/>
+      <c r="J3" s="47">
+        <v>240</v>
+      </c>
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1398,7 +1616,7 @@
         <v>104</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>97</v>
@@ -1430,7 +1648,7 @@
         <v>105</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>97</v>
@@ -1462,7 +1680,7 @@
         <v>106</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>97</v>
@@ -1491,7 +1709,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>113</v>
@@ -1500,7 +1718,7 @@
         <v>97</v>
       </c>
       <c r="D10" s="19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>87</v>
@@ -1523,7 +1741,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>114</v>
@@ -1532,14 +1750,14 @@
         <v>97</v>
       </c>
       <c r="D11" s="19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="19">
         <f t="shared" si="0"/>
@@ -1555,16 +1773,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D12" s="19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>87</v>
@@ -1587,16 +1805,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D13" s="19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>87</v>
@@ -1619,22 +1837,24 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F14" s="20"/>
-      <c r="G14" s="19"/>
+      <c r="G14" s="19">
+        <v>1</v>
+      </c>
       <c r="H14" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1649,10 +1869,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>97</v>
@@ -1664,7 +1884,9 @@
         <v>87</v>
       </c>
       <c r="F15" s="20"/>
-      <c r="G15" s="19"/>
+      <c r="G15" s="19">
+        <v>3</v>
+      </c>
       <c r="H15" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1679,22 +1901,24 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F16" s="20"/>
-      <c r="G16" s="19"/>
+      <c r="G16" s="19">
+        <v>1</v>
+      </c>
       <c r="H16" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1708,17 +1932,25 @@
       <c r="K16" s="22"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>128</v>
+      </c>
       <c r="C17" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D17" s="19">
+        <v>6</v>
+      </c>
       <c r="E17" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F17" s="20"/>
-      <c r="G17" s="19"/>
+      <c r="G17" s="19">
+        <v>1</v>
+      </c>
       <c r="H17" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1732,17 +1964,25 @@
       <c r="K17" s="22"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>129</v>
+      </c>
       <c r="C18" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D18" s="19">
+        <v>6</v>
+      </c>
       <c r="E18" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F18" s="20"/>
-      <c r="G18" s="19"/>
+      <c r="G18" s="19">
+        <v>1</v>
+      </c>
       <c r="H18" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1756,17 +1996,25 @@
       <c r="K18" s="22"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>134</v>
+      </c>
       <c r="C19" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D19" s="19">
+        <v>2</v>
+      </c>
       <c r="E19" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F19" s="20"/>
-      <c r="G19" s="19"/>
+      <c r="G19" s="19">
+        <v>1</v>
+      </c>
       <c r="H19" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1780,17 +2028,25 @@
       <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="C20" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D20" s="19">
+        <v>2</v>
+      </c>
       <c r="E20" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F20" s="20"/>
-      <c r="G20" s="19"/>
+      <c r="G20" s="19">
+        <v>1</v>
+      </c>
       <c r="H20" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1804,17 +2060,25 @@
       <c r="K20" s="22"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>138</v>
+      </c>
       <c r="C21" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D21" s="19">
+        <v>2</v>
+      </c>
       <c r="E21" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F21" s="20"/>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19">
+        <v>1</v>
+      </c>
       <c r="H21" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1828,17 +2092,25 @@
       <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>146</v>
+      </c>
       <c r="C22" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D22" s="19">
+        <v>1</v>
+      </c>
       <c r="E22" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F22" s="20"/>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19">
+        <v>3</v>
+      </c>
       <c r="H22" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1852,17 +2124,25 @@
       <c r="K22" s="22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>142</v>
+      </c>
       <c r="C23" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D23" s="19">
+        <v>6</v>
+      </c>
       <c r="E23" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F23" s="20"/>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19">
+        <v>1</v>
+      </c>
       <c r="H23" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1876,17 +2156,25 @@
       <c r="K23" s="22"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>143</v>
+      </c>
       <c r="C24" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D24" s="19">
+        <v>6</v>
+      </c>
       <c r="E24" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F24" s="20"/>
-      <c r="G24" s="19"/>
+      <c r="G24" s="19">
+        <v>1</v>
+      </c>
       <c r="H24" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1900,17 +2188,25 @@
       <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>144</v>
+      </c>
       <c r="C25" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D25" s="19">
+        <v>6</v>
+      </c>
       <c r="E25" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F25" s="20"/>
-      <c r="G25" s="19"/>
+      <c r="G25" s="19">
+        <v>1</v>
+      </c>
       <c r="H25" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1924,17 +2220,25 @@
       <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>148</v>
+      </c>
       <c r="C26" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D26" s="19">
+        <v>1</v>
+      </c>
       <c r="E26" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F26" s="20"/>
-      <c r="G26" s="19"/>
+      <c r="G26" s="19">
+        <v>3</v>
+      </c>
       <c r="H26" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1948,17 +2252,25 @@
       <c r="K26" s="22"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>152</v>
+      </c>
       <c r="C27" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D27" s="19">
+        <v>4</v>
+      </c>
       <c r="E27" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F27" s="20"/>
-      <c r="G27" s="19"/>
+      <c r="G27" s="19">
+        <v>1</v>
+      </c>
       <c r="H27" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1972,17 +2284,25 @@
       <c r="K27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>153</v>
+      </c>
       <c r="C28" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D28" s="19">
+        <v>4</v>
+      </c>
       <c r="E28" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F28" s="20"/>
-      <c r="G28" s="19"/>
+      <c r="G28" s="19">
+        <v>1</v>
+      </c>
       <c r="H28" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1996,17 +2316,25 @@
       <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>154</v>
+      </c>
       <c r="C29" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="D29" s="19">
+        <v>4</v>
+      </c>
       <c r="E29" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F29" s="20"/>
-      <c r="G29" s="19"/>
+      <c r="G29" s="19">
+        <v>1</v>
+      </c>
       <c r="H29" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2020,23 +2348,31 @@
       <c r="K29" s="22"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="18"/>
+      <c r="A30" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>121</v>
+      </c>
       <c r="C30" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D30" s="19">
+        <v>3</v>
+      </c>
       <c r="E30" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F30" s="20"/>
-      <c r="G30" s="19"/>
+      <c r="G30" s="19">
+        <v>1</v>
+      </c>
       <c r="H30" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J30" s="22" t="s">
         <v>71</v>
@@ -2044,23 +2380,31 @@
       <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="C31" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D31" s="19">
+        <v>2</v>
+      </c>
       <c r="E31" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F31" s="20"/>
-      <c r="G31" s="19"/>
+      <c r="G31" s="19">
+        <v>1</v>
+      </c>
       <c r="H31" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J31" s="22" t="s">
         <v>71</v>
@@ -2068,23 +2412,31 @@
       <c r="K31" s="22"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="18"/>
+      <c r="A32" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>158</v>
+      </c>
       <c r="C32" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D32" s="19">
+        <v>1</v>
+      </c>
       <c r="E32" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F32" s="20"/>
-      <c r="G32" s="19"/>
+      <c r="G32" s="19">
+        <v>1</v>
+      </c>
       <c r="H32" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J32" s="22" t="s">
         <v>71</v>
@@ -2092,23 +2444,31 @@
       <c r="K32" s="22"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="18"/>
+      <c r="A33" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>123</v>
+      </c>
       <c r="C33" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D33" s="19">
+        <v>4</v>
+      </c>
       <c r="E33" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F33" s="20"/>
-      <c r="G33" s="19"/>
+      <c r="G33" s="19">
+        <v>1</v>
+      </c>
       <c r="H33" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J33" s="22" t="s">
         <v>71</v>
@@ -2116,23 +2476,31 @@
       <c r="K33" s="22"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
-      <c r="B34" s="18"/>
+      <c r="A34" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>160</v>
+      </c>
       <c r="C34" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D34" s="19">
+        <v>3</v>
+      </c>
       <c r="E34" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F34" s="20"/>
-      <c r="G34" s="19"/>
+      <c r="G34" s="19">
+        <v>1</v>
+      </c>
       <c r="H34" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J34" s="22" t="s">
         <v>71</v>
@@ -2140,23 +2508,31 @@
       <c r="K34" s="22"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="B35" s="18"/>
+      <c r="A35" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>124</v>
+      </c>
       <c r="C35" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D35" s="19">
+        <v>3</v>
+      </c>
       <c r="E35" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F35" s="20"/>
-      <c r="G35" s="19"/>
+      <c r="G35" s="19">
+        <v>1</v>
+      </c>
       <c r="H35" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J35" s="22" t="s">
         <v>71</v>
@@ -2164,23 +2540,31 @@
       <c r="K35" s="22"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="18"/>
+      <c r="A36" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>162</v>
+      </c>
       <c r="C36" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D36" s="19">
+        <v>3</v>
+      </c>
       <c r="E36" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F36" s="20"/>
-      <c r="G36" s="19"/>
+      <c r="G36" s="19">
+        <v>1</v>
+      </c>
       <c r="H36" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J36" s="22" t="s">
         <v>71</v>
@@ -2188,23 +2572,31 @@
       <c r="K36" s="22"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="B37" s="18"/>
+      <c r="A37" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>164</v>
+      </c>
       <c r="C37" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D37" s="19">
+        <v>4</v>
+      </c>
       <c r="E37" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F37" s="20"/>
-      <c r="G37" s="19"/>
+      <c r="G37" s="19">
+        <v>1</v>
+      </c>
       <c r="H37" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J37" s="22" t="s">
         <v>71</v>
@@ -2212,23 +2604,31 @@
       <c r="K37" s="22"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="18"/>
+      <c r="A38" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>166</v>
+      </c>
       <c r="C38" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D38" s="19">
+        <v>4</v>
+      </c>
       <c r="E38" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F38" s="20"/>
-      <c r="G38" s="19"/>
+      <c r="G38" s="19">
+        <v>1</v>
+      </c>
       <c r="H38" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J38" s="22" t="s">
         <v>71</v>
@@ -2236,23 +2636,31 @@
       <c r="K38" s="22"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="18"/>
+      <c r="A39" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>164</v>
+      </c>
       <c r="C39" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D39" s="19">
+        <v>4</v>
+      </c>
       <c r="E39" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F39" s="20"/>
-      <c r="G39" s="19"/>
+      <c r="G39" s="19">
+        <v>1</v>
+      </c>
       <c r="H39" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J39" s="22" t="s">
         <v>71</v>
@@ -2260,23 +2668,31 @@
       <c r="K39" s="22"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="18"/>
+      <c r="A40" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>169</v>
+      </c>
       <c r="C40" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D40" s="19">
+        <v>4</v>
+      </c>
       <c r="E40" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F40" s="20"/>
-      <c r="G40" s="19"/>
+      <c r="G40" s="19">
+        <v>1</v>
+      </c>
       <c r="H40" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J40" s="22" t="s">
         <v>71</v>
@@ -2284,23 +2700,31 @@
       <c r="K40" s="22"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
+      <c r="A41" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>171</v>
+      </c>
       <c r="C41" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D41" s="19">
+        <v>4</v>
+      </c>
       <c r="E41" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F41" s="20"/>
-      <c r="G41" s="19"/>
+      <c r="G41" s="19">
+        <v>1</v>
+      </c>
       <c r="H41" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J41" s="22" t="s">
         <v>71</v>
@@ -2308,23 +2732,31 @@
       <c r="K41" s="22"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
-      <c r="B42" s="18"/>
+      <c r="A42" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>173</v>
+      </c>
       <c r="C42" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D42" s="19">
+        <v>4</v>
+      </c>
       <c r="E42" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F42" s="20"/>
-      <c r="G42" s="19"/>
+      <c r="G42" s="19">
+        <v>1</v>
+      </c>
       <c r="H42" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J42" s="22" t="s">
         <v>71</v>
@@ -2332,23 +2764,31 @@
       <c r="K42" s="22"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="18"/>
+      <c r="A43" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>175</v>
+      </c>
       <c r="C43" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D43" s="19">
+        <v>4</v>
+      </c>
       <c r="E43" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F43" s="20"/>
-      <c r="G43" s="19"/>
+      <c r="G43" s="19">
+        <v>1</v>
+      </c>
       <c r="H43" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="J43" s="22" t="s">
         <v>71</v>
@@ -2356,23 +2796,31 @@
       <c r="K43" s="22"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="18"/>
+      <c r="A44" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>176</v>
+      </c>
       <c r="C44" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="E44" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F44" s="20"/>
-      <c r="G44" s="19"/>
+      <c r="G44" s="19">
+        <v>1</v>
+      </c>
       <c r="H44" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J44" s="22" t="s">
         <v>71</v>
@@ -2380,23 +2828,31 @@
       <c r="K44" s="22"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
-      <c r="B45" s="18"/>
+      <c r="A45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="C45" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D45" s="19">
+        <v>4</v>
+      </c>
       <c r="E45" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F45" s="20"/>
-      <c r="G45" s="19"/>
+      <c r="G45" s="19">
+        <v>1</v>
+      </c>
       <c r="H45" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="J45" s="22" t="s">
         <v>71</v>
@@ -2404,23 +2860,31 @@
       <c r="K45" s="22"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
-      <c r="B46" s="18"/>
+      <c r="A46" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="C46" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D46" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="E46" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F46" s="20"/>
-      <c r="G46" s="19"/>
+      <c r="G46" s="19">
+        <v>1</v>
+      </c>
       <c r="H46" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J46" s="22" t="s">
         <v>71</v>
@@ -2428,23 +2892,31 @@
       <c r="K46" s="22"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="18"/>
+      <c r="A47" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="C47" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D47" s="19">
+        <v>4</v>
+      </c>
       <c r="E47" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F47" s="20"/>
-      <c r="G47" s="19"/>
+      <c r="G47" s="19">
+        <v>1</v>
+      </c>
       <c r="H47" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="J47" s="22" t="s">
         <v>71</v>
@@ -2452,23 +2924,31 @@
       <c r="K47" s="22"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="B48" s="18"/>
+      <c r="A48" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>183</v>
+      </c>
       <c r="C48" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="E48" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F48" s="20"/>
-      <c r="G48" s="19"/>
+      <c r="G48" s="19">
+        <v>1</v>
+      </c>
       <c r="H48" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J48" s="22" t="s">
         <v>71</v>
@@ -2476,23 +2956,31 @@
       <c r="K48" s="22"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
-      <c r="B49" s="18"/>
+      <c r="A49" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>185</v>
+      </c>
       <c r="C49" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D49" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D49" s="19">
+        <v>4</v>
+      </c>
       <c r="E49" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F49" s="20"/>
-      <c r="G49" s="19"/>
+      <c r="G49" s="19">
+        <v>1</v>
+      </c>
       <c r="H49" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="J49" s="22" t="s">
         <v>71</v>
@@ -2500,23 +2988,31 @@
       <c r="K49" s="22"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18"/>
+      <c r="A50" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>186</v>
+      </c>
       <c r="C50" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D50" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="E50" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F50" s="20"/>
-      <c r="G50" s="19"/>
+      <c r="G50" s="19">
+        <v>1</v>
+      </c>
       <c r="H50" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J50" s="22" t="s">
         <v>71</v>
@@ -2524,23 +3020,31 @@
       <c r="K50" s="22"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="18"/>
+      <c r="A51" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>188</v>
+      </c>
       <c r="C51" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D51" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D51" s="19">
+        <v>4</v>
+      </c>
       <c r="E51" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F51" s="20"/>
-      <c r="G51" s="19"/>
+      <c r="G51" s="19">
+        <v>1</v>
+      </c>
       <c r="H51" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="J51" s="22" t="s">
         <v>71</v>
@@ -2548,23 +3052,31 @@
       <c r="K51" s="22"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
-      <c r="B52" s="18"/>
+      <c r="A52" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="C52" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="E52" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F52" s="20"/>
-      <c r="G52" s="19"/>
+      <c r="G52" s="19">
+        <v>1</v>
+      </c>
       <c r="H52" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J52" s="22" t="s">
         <v>71</v>
@@ -2572,23 +3084,31 @@
       <c r="K52" s="22"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="18"/>
+      <c r="A53" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>191</v>
+      </c>
       <c r="C53" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D53" s="19">
+        <v>4</v>
+      </c>
       <c r="E53" s="21" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F53" s="20"/>
-      <c r="G53" s="19"/>
+      <c r="G53" s="19">
+        <v>1</v>
+      </c>
       <c r="H53" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="J53" s="22" t="s">
         <v>71</v>
@@ -2596,23 +3116,31 @@
       <c r="K53" s="22"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="18"/>
+      <c r="A54" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>192</v>
+      </c>
       <c r="C54" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="E54" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F54" s="20"/>
-      <c r="G54" s="19"/>
+      <c r="G54" s="19">
+        <v>1</v>
+      </c>
       <c r="H54" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J54" s="22" t="s">
         <v>71</v>
@@ -2866,7 +3394,7 @@
       </c>
       <c r="D66" s="29">
         <f>SUM(D6:D64)</f>
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>78</v>
@@ -2911,7 +3439,9 @@
         <f>E70/21</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G70" s="40"/>
+      <c r="G70" s="40">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
@@ -2926,7 +3456,9 @@
         <f>E71/28</f>
         <v>0</v>
       </c>
-      <c r="G71" s="40"/>
+      <c r="G71" s="40">
+        <v>2</v>
+      </c>
       <c r="P71" s="13"/>
     </row>
     <row r="72" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2942,7 +3474,9 @@
         <f>E72</f>
         <v>0</v>
       </c>
-      <c r="G72" s="41"/>
+      <c r="G72" s="41">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="16">

</xml_diff>

<commit_message>
Update work units worksheet for budget revision.
</commit_message>
<xml_diff>
--- a/assets/Work Units.xlsx
+++ b/assets/Work Units.xlsx
@@ -9,28 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="26380" windowHeight="20180"/>
+    <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="31560"/>
   </bookViews>
   <sheets>
     <sheet name="Course List" sheetId="1" r:id="rId1"/>
     <sheet name="Tables" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Course List'!$A$1:$J$72</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Course List'!$E$70:$E$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Course List'!$A$1:$J$78</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Course List'!$E$76:$E$77</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Course List'!$G$73</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Course List'!$G$73</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Course List'!$G$73</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Course List'!$G$79</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Course List'!$G$79</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Course List'!$G$79</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Course List'!$E$72</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Course List'!$E$78</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Course List'!$G$66</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Course List'!$G$66</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Course List'!$G$66</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Course List'!$G$72</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Course List'!$G$72</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Course List'!$G$72</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="198">
   <si>
     <t>Agriculture</t>
   </si>
@@ -380,15 +380,6 @@
     <t>SE 103</t>
   </si>
   <si>
-    <t>SE 111</t>
-  </si>
-  <si>
-    <t>SE 112</t>
-  </si>
-  <si>
-    <t>SE 113</t>
-  </si>
-  <si>
     <t>Introduction to Software Engineering I</t>
   </si>
   <si>
@@ -401,24 +392,9 @@
     <t>Professional Seminar</t>
   </si>
   <si>
-    <t>Apprenticeship I</t>
-  </si>
-  <si>
-    <t>Creative Problem Solving with Code I</t>
-  </si>
-  <si>
-    <t>Creative Problem Solving with Code II</t>
-  </si>
-  <si>
-    <t>Creative Problem Solving with Code III</t>
-  </si>
-  <si>
     <t>SE 107</t>
   </si>
   <si>
-    <t>SE 110</t>
-  </si>
-  <si>
     <t>WR 121</t>
   </si>
   <si>
@@ -434,12 +410,6 @@
     <t>Public Speaking</t>
   </si>
   <si>
-    <t>SE 211</t>
-  </si>
-  <si>
-    <t>SE 212</t>
-  </si>
-  <si>
     <t>Data Science Engineering I</t>
   </si>
   <si>
@@ -449,9 +419,6 @@
     <t>Data Science Engineering III</t>
   </si>
   <si>
-    <t>SE 213</t>
-  </si>
-  <si>
     <t>SE 210</t>
   </si>
   <si>
@@ -506,15 +473,6 @@
     <t>Apprenticeship IV</t>
   </si>
   <si>
-    <t>SE 411</t>
-  </si>
-  <si>
-    <t>SE 412</t>
-  </si>
-  <si>
-    <t>SE 413</t>
-  </si>
-  <si>
     <t>Business of Software I</t>
   </si>
   <si>
@@ -593,12 +551,6 @@
     <t>3 or 4</t>
   </si>
   <si>
-    <t>CS 271</t>
-  </si>
-  <si>
-    <t>Computer Architecture &amp; Assembly Language</t>
-  </si>
-  <si>
     <t>Cultural Diversity</t>
   </si>
   <si>
@@ -629,16 +581,76 @@
     <t>Synthesis, Contemporary Global Issues</t>
   </si>
   <si>
-    <t>CS XXX</t>
-  </si>
-  <si>
-    <t>(Upper-division CS elective)</t>
-  </si>
-  <si>
     <t>Social Process &amp; Intitutions</t>
   </si>
   <si>
     <t>COMM 111</t>
+  </si>
+  <si>
+    <t>SE 201</t>
+  </si>
+  <si>
+    <t>SE 202</t>
+  </si>
+  <si>
+    <t>SE 203</t>
+  </si>
+  <si>
+    <t>SE 401</t>
+  </si>
+  <si>
+    <t>SE 402</t>
+  </si>
+  <si>
+    <t>SE 403</t>
+  </si>
+  <si>
+    <t>SUS 101</t>
+  </si>
+  <si>
+    <t>Intro to Environmental Science</t>
+  </si>
+  <si>
+    <t>GEOG 360</t>
+  </si>
+  <si>
+    <t>Geographic Information Systems</t>
+  </si>
+  <si>
+    <t>SUS 103</t>
+  </si>
+  <si>
+    <t>Introduction to Climate Change</t>
+  </si>
+  <si>
+    <t>MTH 245</t>
+  </si>
+  <si>
+    <t>Math for Mgmt, Life &amp; Soc. Science</t>
+  </si>
+  <si>
+    <t>SOIL 205</t>
+  </si>
+  <si>
+    <t>SOIL 206</t>
+  </si>
+  <si>
+    <t>Soil Science</t>
+  </si>
+  <si>
+    <t>Soil Science Lab</t>
+  </si>
+  <si>
+    <t>MTH 251</t>
+  </si>
+  <si>
+    <t>Differential Calculus</t>
+  </si>
+  <si>
+    <t>WR 303</t>
+  </si>
+  <si>
+    <t>Writing for the Web</t>
   </si>
 </sst>
 </file>
@@ -1464,11 +1476,11 @@
     <tabColor theme="5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1616,13 +1628,13 @@
         <v>104</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D7" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>87</v>
@@ -1648,13 +1660,13 @@
         <v>105</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>87</v>
@@ -1664,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="19">
-        <f t="shared" ref="H8:H64" si="0">IF(I8="Select",1,0)</f>
+        <f>IF(I8="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I8" s="21" t="s">
@@ -1680,13 +1692,13 @@
         <v>106</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D9" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>87</v>
@@ -1696,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I9="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I9" s="21" t="s">
@@ -1709,16 +1721,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D10" s="19">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>87</v>
@@ -1728,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I10="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I10" s="21" t="s">
@@ -1741,26 +1753,26 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D11" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I11="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I11" s="21" t="s">
@@ -1773,16 +1785,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D12" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>87</v>
@@ -1792,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I12="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I12" s="21" t="s">
@@ -1805,16 +1817,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D13" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>87</v>
@@ -1824,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I13="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I13" s="21" t="s">
@@ -1837,26 +1849,26 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="19">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H14" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I14="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I14" s="21" t="s">
@@ -1869,26 +1881,26 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>131</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>132</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D15" s="19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H15" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I15="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I15" s="21" t="s">
@@ -1901,16 +1913,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>87</v>
@@ -1920,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I16="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I16" s="21" t="s">
@@ -1933,16 +1945,16 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D17" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>87</v>
@@ -1952,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I17="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I17" s="21" t="s">
@@ -1965,26 +1977,26 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D18" s="19">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I18="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I18" s="21" t="s">
@@ -1997,10 +2009,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>97</v>
@@ -2016,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I19="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I19" s="21" t="s">
@@ -2029,10 +2041,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>97</v>
@@ -2048,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I20="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I20" s="21" t="s">
@@ -2061,10 +2073,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>97</v>
@@ -2080,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I21="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I21" s="21" t="s">
@@ -2093,26 +2105,26 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D22" s="19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H22" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I22="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I22" s="21" t="s">
@@ -2125,16 +2137,16 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>142</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D23" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>87</v>
@@ -2144,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I23="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I23" s="21" t="s">
@@ -2157,16 +2169,16 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>140</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D24" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>87</v>
@@ -2176,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I24="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I24" s="21" t="s">
@@ -2189,26 +2201,26 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D25" s="19">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H25" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I25="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I25" s="21" t="s">
@@ -2221,30 +2233,30 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="D26" s="19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(I26="Select",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J26" s="22" t="s">
         <v>71</v>
@@ -2253,16 +2265,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="D27" s="19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27" s="21" t="s">
         <v>87</v>
@@ -2272,11 +2284,11 @@
         <v>1</v>
       </c>
       <c r="H27" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(I27="Select",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J27" s="22" t="s">
         <v>71</v>
@@ -2285,16 +2297,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="D28" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>87</v>
@@ -2304,11 +2316,11 @@
         <v>1</v>
       </c>
       <c r="H28" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(I28="Select",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J28" s="22" t="s">
         <v>71</v>
@@ -2317,16 +2329,16 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="D29" s="19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>87</v>
@@ -2336,11 +2348,11 @@
         <v>1</v>
       </c>
       <c r="H29" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(I29="Select",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J29" s="22" t="s">
         <v>71</v>
@@ -2349,16 +2361,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>87</v>
@@ -2368,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I30="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I30" s="21" t="s">
@@ -2381,16 +2393,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D31" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="21" t="s">
         <v>87</v>
@@ -2400,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I31="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I31" s="21" t="s">
@@ -2413,16 +2425,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D32" s="19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>87</v>
@@ -2432,11 +2444,11 @@
         <v>1</v>
       </c>
       <c r="H32" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I32="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="J32" s="22" t="s">
         <v>71</v>
@@ -2445,10 +2457,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>123</v>
+        <v>187</v>
       </c>
       <c r="C33" s="21" t="s">
         <v>55</v>
@@ -2464,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I33="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I33" s="21" t="s">
@@ -2477,16 +2489,16 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D34" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34" s="21" t="s">
         <v>87</v>
@@ -2496,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I34="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I34" s="21" t="s">
@@ -2509,10 +2521,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>55</v>
@@ -2528,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I35="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I35" s="21" t="s">
@@ -2541,16 +2553,16 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D36" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E36" s="21" t="s">
         <v>87</v>
@@ -2560,11 +2572,11 @@
         <v>1</v>
       </c>
       <c r="H36" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I36="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="J36" s="22" t="s">
         <v>71</v>
@@ -2573,10 +2585,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>55</v>
@@ -2592,11 +2604,11 @@
         <v>1</v>
       </c>
       <c r="H37" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I37="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="J37" s="22" t="s">
         <v>71</v>
@@ -2605,10 +2617,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>55</v>
@@ -2624,11 +2636,11 @@
         <v>1</v>
       </c>
       <c r="H38" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I38="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J38" s="22" t="s">
         <v>71</v>
@@ -2637,10 +2649,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>55</v>
@@ -2656,11 +2668,11 @@
         <v>1</v>
       </c>
       <c r="H39" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I39="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="J39" s="22" t="s">
         <v>71</v>
@@ -2669,10 +2681,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>55</v>
@@ -2688,11 +2700,11 @@
         <v>1</v>
       </c>
       <c r="H40" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I40="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="J40" s="22" t="s">
         <v>71</v>
@@ -2701,16 +2713,16 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C41" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="19">
-        <v>4</v>
+      <c r="D41" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="E41" s="21" t="s">
         <v>87</v>
@@ -2720,11 +2732,11 @@
         <v>1</v>
       </c>
       <c r="H41" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I41="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="J41" s="22" t="s">
         <v>71</v>
@@ -2733,16 +2745,16 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>172</v>
+        <v>99</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="19">
-        <v>4</v>
+      <c r="D42" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="E42" s="21" t="s">
         <v>87</v>
@@ -2752,11 +2764,11 @@
         <v>1</v>
       </c>
       <c r="H42" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I42="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="J42" s="22" t="s">
         <v>71</v>
@@ -2765,10 +2777,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C43" s="21" t="s">
         <v>55</v>
@@ -2784,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I43="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I43" s="21" t="s">
@@ -2797,16 +2809,16 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="19" t="s">
-        <v>177</v>
+      <c r="D44" s="19">
+        <v>3</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>87</v>
@@ -2816,7 +2828,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I44="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I44" s="21" t="s">
@@ -2829,16 +2841,16 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D45" s="19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E45" s="21" t="s">
         <v>87</v>
@@ -2848,11 +2860,11 @@
         <v>1</v>
       </c>
       <c r="H45" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I45="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="J45" s="22" t="s">
         <v>71</v>
@@ -2861,16 +2873,16 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="19" t="s">
-        <v>177</v>
+      <c r="D46" s="19">
+        <v>4</v>
       </c>
       <c r="E46" s="21" t="s">
         <v>87</v>
@@ -2880,11 +2892,11 @@
         <v>1</v>
       </c>
       <c r="H46" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I46="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="J46" s="22" t="s">
         <v>71</v>
@@ -2893,16 +2905,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="19">
-        <v>4</v>
+      <c r="D47" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="E47" s="21" t="s">
         <v>87</v>
@@ -2912,11 +2924,11 @@
         <v>1</v>
       </c>
       <c r="H47" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I47="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="J47" s="22" t="s">
         <v>71</v>
@@ -2925,16 +2937,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="19" t="s">
-        <v>177</v>
+      <c r="D48" s="19">
+        <v>3</v>
       </c>
       <c r="E48" s="21" t="s">
         <v>87</v>
@@ -2944,7 +2956,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I48="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I48" s="21" t="s">
@@ -2957,16 +2969,16 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>184</v>
+        <v>99</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="C49" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="19">
-        <v>4</v>
+      <c r="D49" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="E49" s="21" t="s">
         <v>87</v>
@@ -2976,11 +2988,11 @@
         <v>1</v>
       </c>
       <c r="H49" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I49="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="J49" s="22" t="s">
         <v>71</v>
@@ -2989,16 +3001,16 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="19" t="s">
-        <v>177</v>
+      <c r="D50" s="19">
+        <v>4</v>
       </c>
       <c r="E50" s="21" t="s">
         <v>87</v>
@@ -3008,11 +3020,11 @@
         <v>1</v>
       </c>
       <c r="H50" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I50="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="J50" s="22" t="s">
         <v>71</v>
@@ -3021,10 +3033,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C51" s="21" t="s">
         <v>55</v>
@@ -3033,18 +3045,18 @@
         <v>4</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="19">
         <v>1</v>
       </c>
       <c r="H51" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I51="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="J51" s="22" t="s">
         <v>71</v>
@@ -3053,16 +3065,16 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="19" t="s">
-        <v>177</v>
+      <c r="D52" s="19">
+        <v>4</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>87</v>
@@ -3072,11 +3084,11 @@
         <v>1</v>
       </c>
       <c r="H52" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I52="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="J52" s="22" t="s">
         <v>71</v>
@@ -3085,30 +3097,30 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="19">
-        <v>4</v>
+      <c r="D53" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="19">
         <v>1</v>
       </c>
       <c r="H53" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I53="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="J53" s="22" t="s">
         <v>71</v>
@@ -3117,54 +3129,62 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C54" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="19" t="s">
-        <v>177</v>
+      <c r="D54" s="19">
+        <v>3</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F54" s="20"/>
       <c r="G54" s="19">
         <v>1</v>
       </c>
       <c r="H54" s="19">
-        <f t="shared" si="0"/>
+        <f>IF(I54="Select",1,0)</f>
         <v>0</v>
       </c>
       <c r="I54" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J54" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K54" s="22"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="J54" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="K54" s="22"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18"/>
+      <c r="B55" s="18" t="s">
+        <v>174</v>
+      </c>
       <c r="C55" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D55" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>163</v>
+      </c>
       <c r="E55" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F55" s="20"/>
-      <c r="G55" s="19"/>
+      <c r="G55" s="19">
+        <v>1</v>
+      </c>
       <c r="H55" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(I55="Select",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I55" s="21" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="J55" s="22" t="s">
         <v>71</v>
@@ -3172,23 +3192,31 @@
       <c r="K55" s="22"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="18"/>
+      <c r="A56" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>169</v>
+      </c>
       <c r="C56" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D56" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="D56" s="19">
+        <v>4</v>
+      </c>
       <c r="E56" s="21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F56" s="20"/>
-      <c r="G56" s="19"/>
+      <c r="G56" s="19">
+        <v>1</v>
+      </c>
       <c r="H56" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(I56="Select",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I56" s="21" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="J56" s="22" t="s">
         <v>71</v>
@@ -3208,7 +3236,7 @@
       <c r="F57" s="20"/>
       <c r="G57" s="19"/>
       <c r="H57" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H57:H68" si="0">IF(I57="Select",1,0)</f>
         <v>1</v>
       </c>
       <c r="I57" s="21" t="s">
@@ -3363,253 +3391,277 @@
       </c>
       <c r="K63" s="22"/>
     </row>
-    <row r="64" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F64" s="26"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="17"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="19"/>
+      <c r="E64" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="20"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I64" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="J64" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="K64" s="46"/>
-    </row>
-    <row r="65" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:16" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="12" t="s">
+      <c r="I64" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J64" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K64" s="22"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A65" s="17"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D65" s="19"/>
+      <c r="E65" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="20"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I65" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J65" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K65" s="22"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" s="17"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D66" s="19"/>
+      <c r="E66" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="20"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I66" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J66" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K66" s="22"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A67" s="17"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D67" s="19"/>
+      <c r="E67" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" s="20"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I67" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J67" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K67" s="22"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="17"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D68" s="19"/>
+      <c r="E68" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="20"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I68" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J68" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K68" s="22"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A69" s="17"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" s="20"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19">
+        <f t="shared" ref="H69:H70" si="1">IF(I69="Select",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I69" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J69" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K69" s="22"/>
+    </row>
+    <row r="70" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="23"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" s="25"/>
+      <c r="E70" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="26"/>
+      <c r="G70" s="25"/>
+      <c r="H70" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I70" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="J70" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K70" s="46"/>
+    </row>
+    <row r="71" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:16" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D66" s="29">
-        <f>SUM(D6:D64)</f>
-        <v>160</v>
-      </c>
-      <c r="F66" s="12" t="s">
+      <c r="D72" s="29">
+        <f>SUM(D6:D70)</f>
+        <v>153</v>
+      </c>
+      <c r="F72" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G66" s="11">
-        <f>SUMPRODUCT(F6:F64,G6:G64,H6:H64)</f>
+      <c r="G72" s="11">
+        <f>SUMPRODUCT(F6:F70,G6:G70,H6:H70)</f>
         <v>3.5</v>
       </c>
-      <c r="M66" s="15"/>
-    </row>
-    <row r="67" spans="1:16" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D68" s="37" t="s">
+      <c r="M72" s="15"/>
+    </row>
+    <row r="73" spans="1:16" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D74" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="39"/>
-    </row>
-    <row r="69" spans="1:16" ht="30" x14ac:dyDescent="0.2">
-      <c r="D69" s="4"/>
-      <c r="E69" s="30" t="s">
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
+    </row>
+    <row r="75" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+      <c r="D75" s="4"/>
+      <c r="E75" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="F69" s="31" t="s">
+      <c r="F75" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="G69" s="32" t="s">
+      <c r="G75" s="32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A70" s="5"/>
-      <c r="D70" s="33" t="s">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A76" s="5"/>
+      <c r="D76" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="E70" s="42">
-        <f>SUMIF(E75:E83,"TT",B75:B83)</f>
+      <c r="E76" s="42">
+        <f>SUMIF(E81:E89,"TT",B81:B89)</f>
         <v>3.5</v>
       </c>
-      <c r="F70" s="34">
-        <f>E70/21</f>
+      <c r="F76" s="34">
+        <f>E76/21</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G70" s="40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A71" s="5"/>
-      <c r="D71" s="33" t="s">
+      <c r="G76" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A77" s="5"/>
+      <c r="D77" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="E71" s="42">
-        <f>SUMIF(E75:E83,"Instructor",B75:B83)</f>
-        <v>0</v>
-      </c>
-      <c r="F71" s="34">
-        <f>E71/28</f>
-        <v>0</v>
-      </c>
-      <c r="G71" s="40">
+      <c r="E77" s="42">
+        <f>SUMIF(E81:E89,"Instructor",B81:B89)</f>
+        <v>0</v>
+      </c>
+      <c r="F77" s="34">
+        <f>E77/28</f>
+        <v>0</v>
+      </c>
+      <c r="G77" s="40">
         <v>2</v>
       </c>
-      <c r="P71" s="13"/>
-    </row>
-    <row r="72" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="D72" s="35" t="s">
+      <c r="P77" s="13"/>
+    </row>
+    <row r="78" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="D78" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="E72" s="43">
-        <f>G66-E70-E71</f>
-        <v>0</v>
-      </c>
-      <c r="F72" s="36">
-        <f>E72</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="16">
-        <f t="shared" ref="A75:A83" si="1">C75/D75</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="B75" s="14">
-        <f>IF(G66=3.5,3.5,IF(A75&lt;0.5,0,IF(AND(A75&gt;=0.5,A75&lt;=1),C75,D75)))</f>
-        <v>3.5</v>
-      </c>
-      <c r="C75">
-        <f>G66</f>
-        <v>3.5</v>
-      </c>
-      <c r="D75">
-        <v>21</v>
-      </c>
-      <c r="E75" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B76" s="14">
-        <f t="shared" ref="B76:B83" si="2">IF(B75=0,0,IF(A76&lt;0.5,0,IF(AND(A76&gt;=0.5,A76&lt;=1),C76,D76)))</f>
-        <v>0</v>
-      </c>
-      <c r="C76">
-        <f>G66-B75</f>
-        <v>0</v>
-      </c>
-      <c r="D76">
-        <v>28</v>
-      </c>
-      <c r="E76" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B77" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C77">
-        <f>G66-B75-B76</f>
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <v>21</v>
-      </c>
-      <c r="E77" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B78" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C78">
-        <f>G66-B75-B76-B77</f>
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>28</v>
-      </c>
-      <c r="E78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B79" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C79">
-        <f>G66-B75-B76-B77-B78</f>
-        <v>0</v>
-      </c>
-      <c r="D79">
-        <v>21</v>
-      </c>
-      <c r="E79" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B80" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C80">
-        <f>G66-B75-B76-B77-B78-B79</f>
-        <v>0</v>
-      </c>
-      <c r="D80">
-        <v>28</v>
-      </c>
-      <c r="E80" t="s">
-        <v>80</v>
+      <c r="E78" s="43">
+        <f>G72-E76-E77</f>
+        <v>0</v>
+      </c>
+      <c r="F78" s="36">
+        <f>E78</f>
+        <v>0</v>
+      </c>
+      <c r="G78" s="41">
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="A81:A89" si="2">C81/D81</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="B81" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>IF(G72=3.5,3.5,IF(A81&lt;0.5,0,IF(AND(A81&gt;=0.5,A81&lt;=1),C81,D81)))</f>
+        <v>3.5</v>
       </c>
       <c r="C81">
-        <f>G66-B75-B76-B77-B78-B79-B80</f>
-        <v>0</v>
+        <f>G72</f>
+        <v>3.5</v>
       </c>
       <c r="D81">
         <v>21</v>
@@ -3620,15 +3672,15 @@
     </row>
     <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="B82" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B82:B89" si="3">IF(B81=0,0,IF(A82&lt;0.5,0,IF(AND(A82&gt;=0.5,A82&lt;=1),C82,D82)))</f>
         <v>0</v>
       </c>
       <c r="C82">
-        <f>G66-B75-B76-B77-B78-B79-B80-B81</f>
+        <f>G72-B81</f>
         <v>0</v>
       </c>
       <c r="D82">
@@ -3640,21 +3692,141 @@
     </row>
     <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="B83" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C83">
-        <f>G66-B75-B76-B77-B78-B79-B80-B81-B82</f>
+        <f>G72-B81-B82</f>
         <v>0</v>
       </c>
       <c r="D83">
         <v>21</v>
       </c>
       <c r="E83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B84" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <f>G72-B81-B82-B83</f>
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>28</v>
+      </c>
+      <c r="E84" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B85" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <f>G72-B81-B82-B83-B84</f>
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>21</v>
+      </c>
+      <c r="E85" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B86" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <f>G72-B81-B82-B83-B84-B85</f>
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>28</v>
+      </c>
+      <c r="E86" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B87" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <f>G72-B81-B82-B83-B84-B85-B86</f>
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>21</v>
+      </c>
+      <c r="E87" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B88" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <f>G72-B81-B82-B83-B84-B85-B86-B87</f>
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>28</v>
+      </c>
+      <c r="E88" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B89" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <f>G72-B81-B82-B83-B84-B85-B86-B87-B88</f>
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>21</v>
+      </c>
+      <c r="E89" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3675,19 +3847,19 @@
           <x14:formula1>
             <xm:f>Tables!$D$1:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E7:E64</xm:sqref>
+          <xm:sqref>E7:E70</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$E$1:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C64</xm:sqref>
+          <xm:sqref>C7:C70</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$A$1:$A$72</xm:f>
           </x14:formula1>
-          <xm:sqref>I7:J64</xm:sqref>
+          <xm:sqref>I7:J70</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>